<commit_message>
9No Sara Khal uploaded
9No Sara Khal uploaded
</commit_message>
<xml_diff>
--- a/Satakhira_DIV_I/FY_23_24/Khal/Khal Data Pol-15/Satkhira all Data/Khal_Hydrologic_Calculation.xlsx
+++ b/Satakhira_DIV_I/FY_23_24/Khal/Khal Data Pol-15/Satkhira all Data/Khal_Hydrologic_Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Design-Circle-8\Satakhira_DIV_I\FY_23_24\Khal\Khal Data Pol-15\Satkhira all Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBA12FA-85D5-4D2D-9E85-12BA79C6F1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089BF8B0-747B-4DC1-8AA5-638B40AF5A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,12 +123,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -158,13 +164,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -449,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:R5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,133 +663,133 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>1949843.923</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <f t="shared" si="0"/>
         <v>194.9843923</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <f t="shared" si="1"/>
         <v>0.75283549150579154</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="5">
         <v>2.298</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5">
         <f t="shared" si="2"/>
         <v>1.4282162834058423</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="5">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="5">
         <f t="shared" si="3"/>
         <v>24.164921398960541</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="5">
         <v>-0.4</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="5">
         <f t="shared" si="4"/>
         <v>0.68682537889864859</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="6">
         <v>135</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="5">
         <v>0.73</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="5">
         <f t="shared" si="5"/>
         <v>98.55</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="5">
         <f t="shared" si="6"/>
         <v>59.129999999999995</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="5">
         <f t="shared" si="7"/>
         <v>99.741984654277076</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="5">
         <f t="shared" si="8"/>
         <v>75.089306040965795</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="5">
         <f t="shared" si="9"/>
         <v>2.1271758085259433</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5" s="4">
         <v>9</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>7322401.0159999998</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <f t="shared" si="0"/>
         <v>732.2401016</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="5">
         <f t="shared" si="1"/>
         <v>2.8271818594594595</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="5">
         <v>4.0170000000000003</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="5">
         <f t="shared" si="2"/>
         <v>2.4965817277812308</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="5">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="5">
         <f t="shared" si="3"/>
         <v>33.784420294133085</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="5">
         <v>-0.4</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="5">
         <f t="shared" si="4"/>
         <v>0.65052431745945938</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="6">
         <v>135</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="5">
         <v>0.73</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="5">
         <f t="shared" si="5"/>
         <v>98.55</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="5">
         <f t="shared" si="6"/>
         <v>59.129999999999995</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="5">
         <f t="shared" si="7"/>
         <v>97.595502891377834</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="5">
         <f t="shared" si="8"/>
         <v>275.92023533932667</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="5">
         <f t="shared" si="9"/>
         <v>7.8164372617372999</v>
       </c>

</xml_diff>